<commit_message>
finalizing and cleaning code
</commit_message>
<xml_diff>
--- a/A1_Experiment_Sheet.xlsx
+++ b/A1_Experiment_Sheet.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://staffusm-my.sharepoint.com/personal/jasyliew_usm_my/Documents/USM/Teaching/Semester 2 2020/CDS503/Assignments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CDS503\Assignment 1\Depression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{9C8F0284-11F4-4DF9-9189-2EDCDE6E0E60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{823D1B38-5C02-415C-BDAD-5376EE117634}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4EB02D-3AC5-4B7E-8E87-26BCB246FC77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0EC0D16C-C842-470A-AD01-3437D2892592}"/>
+    <workbookView xWindow="525" yWindow="1080" windowWidth="23550" windowHeight="9030" xr2:uid="{0EC0D16C-C842-470A-AD01-3437D2892592}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment_Results" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Experiment_Results!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Experiment_Results!$A$1:$H$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
   <si>
     <t>Feature Representation</t>
   </si>
@@ -77,9 +77,6 @@
     <t>DummyClassifier</t>
   </si>
   <si>
-    <t>strategy=uniform</t>
-  </si>
-  <si>
     <t>Validation Accuracy</t>
   </si>
   <si>
@@ -90,13 +87,55 @@
   </si>
   <si>
     <t>Validation F1 (Weighted Avg)</t>
+  </si>
+  <si>
+    <t>K-Nearest Neighbor</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>Decision Tree</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>cv=10, kernel='rbf', C=1</t>
+  </si>
+  <si>
+    <t>cv=10</t>
+  </si>
+  <si>
+    <t>cv=10, criterion='gini', max_depth=2</t>
+  </si>
+  <si>
+    <t>cv=5, k=27, p=2</t>
+  </si>
+  <si>
+    <t>cv=10, kernel='poly', C=1</t>
+  </si>
+  <si>
+    <t>cv=10, criterion='gini', max_depth=3</t>
+  </si>
+  <si>
+    <t>Naïve Bayes GaussianNB()</t>
+  </si>
+  <si>
+    <t>Naïve Bayes MultinomialNB()</t>
+  </si>
+  <si>
+    <t>cv=10 strategy=uniform</t>
+  </si>
+  <si>
+    <t>cv=10, strategy=uniform</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,12 +147,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -131,7 +164,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,6 +174,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -157,11 +196,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,25 +530,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21B9B9AE-3221-4C5E-9101-420F4A4AA422}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.21875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.21875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="36" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -522,48 +563,305 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.54</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.49</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.49</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.64</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.64</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.64</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.64</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.67</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.64</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.69</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.69</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0.69</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0.69</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{C16A36FD-C2FB-404E-B39A-6801620F86E4}"/>
+  <autoFilter ref="A1:H11" xr:uid="{C16A36FD-C2FB-404E-B39A-6801620F86E4}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H11">
+      <sortCondition ref="A1:A11"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B3864872A4218E41B6727955A53CA831" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1954879c5e13ef2e6734fd8b475519ba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c275662b-d2ec-4adf-b3dc-ab2da4ea4bdb" xmlns:ns4="a25d2d83-ddc7-4b30-a263-1f552d167900" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f073ca29401fa9a2d9fdf2f43f14f5a6" ns3:_="" ns4:_="">
     <xsd:import namespace="c275662b-d2ec-4adf-b3dc-ab2da4ea4bdb"/>
@@ -786,22 +1084,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC11B67F-8F8E-4754-AD61-DF467A1D7806}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{597094D5-6E03-4148-99B9-8235D6329E5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62142156-2A69-4FF3-A327-BCAC8615267D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -818,21 +1118,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{597094D5-6E03-4148-99B9-8235D6329E5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC11B67F-8F8E-4754-AD61-DF467A1D7806}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>